<commit_message>
Labs updated for Fall 2018
</commit_message>
<xml_diff>
--- a/StudentGuideModule1/what_labs_to_include/131 lab list for 2018fall.xlsx
+++ b/StudentGuideModule1/what_labs_to_include/131 lab list for 2018fall.xlsx
@@ -180,7 +180,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="190">
   <si>
     <t>1 Music to Our Ears: Standing Waves in Strings 7</t>
   </si>
@@ -751,6 +751,9 @@
   </si>
   <si>
     <t xml:space="preserve">Total # users </t>
+  </si>
+  <si>
+    <t>Obsolete; we use Capstone.</t>
   </si>
 </sst>
 </file>
@@ -1634,7 +1637,49 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="9">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCDFFCD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF99FF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCDFFCD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF99FF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1967,8 +2012,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB112"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S2" sqref="S2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U69" sqref="U69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2087,13 +2132,19 @@
         <v>1</v>
       </c>
       <c r="M2" s="59"/>
-      <c r="N2" s="68"/>
+      <c r="N2" s="68">
+        <v>1</v>
+      </c>
       <c r="O2" s="59"/>
-      <c r="P2" s="59"/>
-      <c r="Q2" s="59"/>
+      <c r="P2" s="59">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="59">
+        <v>1</v>
+      </c>
       <c r="R2" s="55"/>
       <c r="S2" s="75">
-        <f t="shared" ref="S2:S33" si="0">SUM(J2:R2)</f>
+        <f>SUM(N2:R2)</f>
         <v>3</v>
       </c>
       <c r="T2" s="80"/>
@@ -2132,13 +2183,19 @@
         <v>1</v>
       </c>
       <c r="M3" s="60"/>
-      <c r="N3" s="63"/>
+      <c r="N3" s="63">
+        <v>1</v>
+      </c>
       <c r="O3" s="60"/>
-      <c r="P3" s="60"/>
-      <c r="Q3" s="60"/>
+      <c r="P3" s="60">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="60">
+        <v>1</v>
+      </c>
       <c r="R3" s="60"/>
       <c r="S3" s="76">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="S3:S66" si="0">SUM(N3:R3)</f>
         <v>3</v>
       </c>
       <c r="T3" s="80"/>
@@ -2186,13 +2243,19 @@
         <v>1</v>
       </c>
       <c r="N4" s="36"/>
-      <c r="O4" s="36"/>
-      <c r="P4" s="36"/>
-      <c r="Q4" s="36"/>
+      <c r="O4" s="36">
+        <v>1</v>
+      </c>
+      <c r="P4" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="Q4" s="36">
+        <v>1</v>
+      </c>
       <c r="R4" s="36"/>
       <c r="S4" s="77">
         <f t="shared" si="0"/>
-        <v>3.5</v>
+        <v>2.5</v>
       </c>
       <c r="T4" s="5"/>
       <c r="U4" s="5"/>
@@ -2221,7 +2284,7 @@
       <c r="R5" s="34"/>
       <c r="S5" s="77">
         <f t="shared" si="0"/>
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="T5" s="5"/>
       <c r="U5" s="5"/>
@@ -2355,10 +2418,16 @@
       <c r="N9" s="36">
         <v>1</v>
       </c>
+      <c r="P9" s="36">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="36">
+        <v>1</v>
+      </c>
       <c r="R9" s="34"/>
       <c r="S9" s="77">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="T9" s="5"/>
       <c r="U9" s="5"/>
@@ -2402,10 +2471,16 @@
       <c r="N10" s="36">
         <v>1</v>
       </c>
+      <c r="P10" s="36">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="36">
+        <v>1</v>
+      </c>
       <c r="R10" s="34"/>
       <c r="S10" s="77">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="T10" s="5"/>
       <c r="U10" s="5"/>
@@ -2444,12 +2519,18 @@
         <v>1</v>
       </c>
       <c r="N11" s="36">
-        <v>0.5</v>
+        <v>1</v>
+      </c>
+      <c r="P11" s="36">
+        <v>0.75</v>
+      </c>
+      <c r="Q11" s="36">
+        <v>1</v>
       </c>
       <c r="R11" s="34"/>
       <c r="S11" s="77">
         <f t="shared" si="0"/>
-        <v>3.25</v>
+        <v>2.75</v>
       </c>
       <c r="T11" s="5"/>
       <c r="U11" s="42" t="s">
@@ -2476,13 +2557,10 @@
         <v>0</v>
       </c>
       <c r="M12" s="36"/>
-      <c r="N12" s="36">
-        <v>0.5</v>
-      </c>
       <c r="R12" s="34"/>
       <c r="S12" s="77">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="T12" s="15"/>
       <c r="U12" s="44">
@@ -2525,10 +2603,16 @@
       <c r="M13" s="36">
         <v>1</v>
       </c>
+      <c r="P13" s="36">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="36">
+        <v>1</v>
+      </c>
       <c r="R13" s="34"/>
       <c r="S13" s="77">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="T13" s="5"/>
       <c r="U13" s="33"/>
@@ -2569,10 +2653,16 @@
       <c r="N14" s="36">
         <v>1</v>
       </c>
+      <c r="P14" s="36">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="36">
+        <v>1</v>
+      </c>
       <c r="R14" s="34"/>
       <c r="S14" s="77">
         <f t="shared" si="0"/>
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="T14" s="5"/>
       <c r="U14" s="1" t="s">
@@ -2633,13 +2723,16 @@
         <v>0</v>
       </c>
       <c r="M16" s="36"/>
-      <c r="N16" s="36">
+      <c r="O16" s="36">
+        <v>1</v>
+      </c>
+      <c r="P16" s="36">
         <v>0.5</v>
       </c>
       <c r="R16" s="34"/>
       <c r="S16" s="77">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
       <c r="T16" s="5"/>
       <c r="U16" s="18" t="s">
@@ -2673,12 +2766,16 @@
         <v>0.75</v>
       </c>
       <c r="M17" s="36"/>
-      <c r="R17" s="34">
-        <v>1</v>
-      </c>
+      <c r="N17" s="36">
+        <v>1</v>
+      </c>
+      <c r="Q17" s="36">
+        <v>1</v>
+      </c>
+      <c r="R17" s="34"/>
       <c r="S17" s="77">
         <f t="shared" si="0"/>
-        <v>2.25</v>
+        <v>2</v>
       </c>
       <c r="T17" s="5"/>
       <c r="U17" s="18" t="s">
@@ -2726,10 +2823,16 @@
       <c r="N18" s="36">
         <v>1</v>
       </c>
+      <c r="P18" s="36">
+        <v>1</v>
+      </c>
+      <c r="Q18" s="36">
+        <v>1</v>
+      </c>
       <c r="R18" s="34"/>
       <c r="S18" s="77">
         <f t="shared" si="0"/>
-        <v>4.75</v>
+        <v>3</v>
       </c>
       <c r="T18" s="5"/>
       <c r="U18" s="18" t="s">
@@ -2841,7 +2944,7 @@
       <c r="L22" s="2">
         <v>0</v>
       </c>
-      <c r="N22" s="36">
+      <c r="P22" s="36">
         <v>0.5</v>
       </c>
       <c r="R22" s="34"/>
@@ -2888,15 +2991,15 @@
         <v>0</v>
       </c>
       <c r="V23" s="6">
-        <f>SUMIF(S$2:S$70,"&gt;=" &amp; U23,C$2:C$70)</f>
+        <f t="shared" ref="V23:V31" si="1">SUMIF(S$2:S$70,"&gt;=" &amp; U23,C$2:C$70)</f>
         <v>300</v>
       </c>
       <c r="W23" s="6">
-        <f>SUMIF(S$2:S$70,"&gt;=" &amp; U23,D$2:D$70)</f>
+        <f t="shared" ref="W23:W31" si="2">SUMIF(S$2:S$70,"&gt;=" &amp; U23,D$2:D$70)</f>
         <v>7</v>
       </c>
       <c r="X23" s="8">
-        <f t="shared" ref="X23:X31" si="1">($W$17 + $W$15*V23+$W$16*W23)*(1+W$18+W$19)</f>
+        <f t="shared" ref="X23:X31" si="3">($W$17 + $W$15*V23+$W$16*W23)*(1+W$18+W$19)</f>
         <v>26.130000000000003</v>
       </c>
       <c r="Y23" s="33"/>
@@ -2940,28 +3043,32 @@
         <v>1</v>
       </c>
       <c r="O24" s="36"/>
-      <c r="P24" s="36"/>
-      <c r="Q24" s="36"/>
+      <c r="P24" s="36">
+        <v>1</v>
+      </c>
+      <c r="Q24" s="36">
+        <v>1</v>
+      </c>
       <c r="R24" s="34"/>
       <c r="S24" s="77">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="T24" s="15"/>
       <c r="U24" s="81">
         <v>0.5</v>
       </c>
       <c r="V24" s="6">
-        <f>SUMIF(S$2:S$70,"&gt;=" &amp; U24,C$2:C$70)</f>
-        <v>268</v>
+        <f t="shared" si="1"/>
+        <v>251</v>
       </c>
       <c r="W24" s="6">
-        <f>SUMIF(S$2:S$70,"&gt;=" &amp; U24,D$2:D$70)</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="X24" s="8">
-        <f t="shared" si="1"/>
-        <v>23.66</v>
+        <f t="shared" si="3"/>
+        <v>22.555000000000003</v>
       </c>
       <c r="Y24" s="33"/>
       <c r="Z24" s="33"/>
@@ -2987,26 +3094,35 @@
       <c r="M25" s="20">
         <v>1</v>
       </c>
+      <c r="N25" s="36">
+        <v>1</v>
+      </c>
+      <c r="P25" s="36">
+        <v>1</v>
+      </c>
+      <c r="Q25" s="36">
+        <v>1</v>
+      </c>
       <c r="R25" s="34"/>
       <c r="S25" s="77">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="T25" s="15"/>
       <c r="U25" s="81">
         <v>1</v>
       </c>
       <c r="V25" s="6">
-        <f>SUMIF(S$2:S$70,"&gt;=" &amp; U25,C$2:C$70)</f>
-        <v>244</v>
+        <f t="shared" si="1"/>
+        <v>247</v>
       </c>
       <c r="W25" s="6">
-        <f>SUMIF(S$2:S$70,"&gt;=" &amp; U25,D$2:D$70)</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="X25" s="8">
-        <f t="shared" si="1"/>
-        <v>22.1</v>
+        <f t="shared" si="3"/>
+        <v>22.295000000000005</v>
       </c>
       <c r="Y25" s="33"/>
       <c r="Z25" s="33"/>
@@ -3042,26 +3158,32 @@
       <c r="N26" s="36">
         <v>1</v>
       </c>
+      <c r="P26" s="36">
+        <v>1</v>
+      </c>
+      <c r="Q26" s="36">
+        <v>1</v>
+      </c>
       <c r="R26" s="34"/>
       <c r="S26" s="77">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T26" s="15"/>
       <c r="U26" s="82">
         <v>1.5</v>
       </c>
       <c r="V26" s="31">
-        <f>SUMIF(S$2:S$70,"&gt;=" &amp; U26,C$2:C$70)</f>
-        <v>223</v>
+        <f t="shared" si="1"/>
+        <v>241</v>
       </c>
       <c r="W26" s="31">
-        <f>SUMIF(S$2:S$70,"&gt;=" &amp; U26,D$2:D$70)</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="X26" s="8">
-        <f t="shared" si="1"/>
-        <v>20.734999999999999</v>
+        <f t="shared" si="3"/>
+        <v>21.905000000000001</v>
       </c>
       <c r="Y26" s="33"/>
       <c r="Z26" s="33"/>
@@ -3103,31 +3225,35 @@
         <v>1</v>
       </c>
       <c r="N27" s="35">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="O27" s="35"/>
-      <c r="P27" s="35"/>
-      <c r="Q27" s="35"/>
+      <c r="P27" s="35">
+        <v>1</v>
+      </c>
+      <c r="Q27" s="35">
+        <v>1</v>
+      </c>
       <c r="R27" s="35"/>
       <c r="S27" s="78">
         <f t="shared" si="0"/>
-        <v>4.5</v>
+        <v>3</v>
       </c>
       <c r="T27" s="15"/>
       <c r="U27" s="81">
         <v>2</v>
       </c>
       <c r="V27" s="6">
-        <f>SUMIF(S$2:S$70,"&gt;=" &amp; U27,C$2:C$70)</f>
-        <v>223</v>
+        <f t="shared" si="1"/>
+        <v>232</v>
       </c>
       <c r="W27" s="6">
-        <f>SUMIF(S$2:S$70,"&gt;=" &amp; U27,D$2:D$70)</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="X27" s="8">
-        <f t="shared" si="1"/>
-        <v>20.734999999999999</v>
+        <f t="shared" si="3"/>
+        <v>21.320000000000004</v>
       </c>
     </row>
     <row r="28" spans="1:28" x14ac:dyDescent="0.3">
@@ -3156,26 +3282,35 @@
       <c r="M28" s="20">
         <v>1</v>
       </c>
+      <c r="N28" s="36">
+        <v>1</v>
+      </c>
+      <c r="P28" s="36">
+        <v>0.75</v>
+      </c>
+      <c r="Q28" s="36">
+        <v>1</v>
+      </c>
       <c r="R28" s="34"/>
       <c r="S28" s="77">
         <f t="shared" si="0"/>
-        <v>2.8</v>
+        <v>2.75</v>
       </c>
       <c r="T28" s="15"/>
       <c r="U28" s="81">
         <v>2.5</v>
       </c>
       <c r="V28" s="6">
-        <f>SUMIF(S$2:S$70,"&gt;=" &amp; U28,C$2:C$70)</f>
-        <v>199</v>
+        <f t="shared" si="1"/>
+        <v>192</v>
       </c>
       <c r="W28" s="6">
-        <f>SUMIF(S$2:S$70,"&gt;=" &amp; U28,D$2:D$70)</f>
-        <v>1</v>
+        <f t="shared" si="2"/>
+        <v>6</v>
       </c>
       <c r="X28" s="8">
-        <f t="shared" si="1"/>
-        <v>17.225000000000001</v>
+        <f t="shared" si="3"/>
+        <v>18.720000000000002</v>
       </c>
     </row>
     <row r="29" spans="1:28" x14ac:dyDescent="0.3">
@@ -3195,23 +3330,23 @@
       <c r="R29" s="34"/>
       <c r="S29" s="77">
         <f t="shared" si="0"/>
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="T29" s="15"/>
       <c r="U29" s="81">
         <v>3</v>
       </c>
       <c r="V29" s="6">
-        <f>SUMIF(S$2:S$70,"&gt;=" &amp; U29,C$2:C$70)</f>
-        <v>168</v>
+        <f t="shared" si="1"/>
+        <v>166</v>
       </c>
       <c r="W29" s="6">
-        <f>SUMIF(S$2:S$70,"&gt;=" &amp; U29,D$2:D$70)</f>
-        <v>1</v>
+        <f t="shared" si="2"/>
+        <v>6</v>
       </c>
       <c r="X29" s="8">
-        <f t="shared" si="1"/>
-        <v>15.210000000000003</v>
+        <f t="shared" si="3"/>
+        <v>17.03</v>
       </c>
     </row>
     <row r="30" spans="1:28" x14ac:dyDescent="0.3">
@@ -3241,26 +3376,32 @@
       <c r="N30" s="36">
         <v>1</v>
       </c>
+      <c r="P30" s="36">
+        <v>1</v>
+      </c>
+      <c r="Q30" s="36">
+        <v>1</v>
+      </c>
       <c r="R30" s="34"/>
       <c r="S30" s="77">
         <f t="shared" si="0"/>
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="T30" s="15"/>
       <c r="U30" s="81">
         <v>3.5</v>
       </c>
       <c r="V30" s="6">
-        <f>SUMIF(S$2:S$70,"&gt;=" &amp; U30,C$2:C$70)</f>
-        <v>149</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="W30" s="6">
-        <f>SUMIF(S$2:S$70,"&gt;=" &amp; U30,D$2:D$70)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="X30" s="8">
-        <f t="shared" si="1"/>
-        <v>13.584999999999999</v>
+        <f t="shared" si="3"/>
+        <v>3.9000000000000004</v>
       </c>
     </row>
     <row r="31" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -3295,26 +3436,32 @@
       <c r="N31" s="36">
         <v>1</v>
       </c>
+      <c r="P31" s="36">
+        <v>1</v>
+      </c>
+      <c r="Q31" s="36">
+        <v>1</v>
+      </c>
       <c r="R31" s="34"/>
       <c r="S31" s="77">
         <f t="shared" si="0"/>
-        <v>4.5</v>
+        <v>3</v>
       </c>
       <c r="T31" s="15"/>
       <c r="U31" s="83">
         <v>4</v>
       </c>
       <c r="V31" s="47">
-        <f>SUMIF(S$2:S$70,"&gt;=" &amp; U31,C$2:C$70)</f>
-        <v>122</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="W31" s="47">
-        <f>SUMIF(S$2:S$70,"&gt;=" &amp; U31,D$2:D$70)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="X31" s="9">
-        <f t="shared" si="1"/>
-        <v>11.830000000000002</v>
+        <f t="shared" si="3"/>
+        <v>3.9000000000000004</v>
       </c>
     </row>
     <row r="32" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -3339,12 +3486,16 @@
       <c r="M32" s="36"/>
       <c r="N32" s="36"/>
       <c r="O32" s="36"/>
-      <c r="P32" s="36"/>
-      <c r="Q32" s="36"/>
+      <c r="P32" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="Q32" s="36">
+        <v>1</v>
+      </c>
       <c r="R32" s="34"/>
       <c r="S32" s="77">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="T32" s="15"/>
       <c r="U32" s="3"/>
@@ -3383,10 +3534,16 @@
       <c r="N33" s="36">
         <v>1</v>
       </c>
+      <c r="P33" s="36">
+        <v>1</v>
+      </c>
+      <c r="Q33" s="36">
+        <v>1</v>
+      </c>
       <c r="R33" s="34"/>
       <c r="S33" s="77">
         <f t="shared" si="0"/>
-        <v>4.5</v>
+        <v>3</v>
       </c>
       <c r="T33" s="15"/>
     </row>
@@ -3410,10 +3567,16 @@
       <c r="M34" s="36">
         <v>1</v>
       </c>
+      <c r="P34" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="Q34" s="36">
+        <v>1</v>
+      </c>
       <c r="R34" s="34"/>
       <c r="S34" s="77">
-        <f t="shared" ref="S34:S66" si="2">SUM(J34:R34)</f>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>1.5</v>
       </c>
       <c r="T34" s="15"/>
     </row>
@@ -3446,10 +3609,16 @@
       <c r="N35" s="36">
         <v>1</v>
       </c>
+      <c r="P35" s="36">
+        <v>1</v>
+      </c>
+      <c r="Q35" s="36">
+        <v>1</v>
+      </c>
       <c r="R35" s="34"/>
       <c r="S35" s="77">
-        <f t="shared" si="2"/>
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="T35" s="15"/>
       <c r="U35" s="84"/>
@@ -3480,10 +3649,19 @@
       <c r="M36" s="36">
         <v>1</v>
       </c>
+      <c r="N36" s="36">
+        <v>1</v>
+      </c>
+      <c r="P36" s="36">
+        <v>1</v>
+      </c>
+      <c r="Q36" s="36">
+        <v>1</v>
+      </c>
       <c r="R36" s="34"/>
       <c r="S36" s="77">
-        <f t="shared" si="2"/>
-        <v>2.5</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="T36" s="15"/>
       <c r="U36" s="84"/>
@@ -3520,12 +3698,16 @@
         <v>0.5</v>
       </c>
       <c r="O37" s="36"/>
-      <c r="P37" s="36"/>
-      <c r="Q37" s="36"/>
+      <c r="P37" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="Q37" s="36">
+        <v>1</v>
+      </c>
       <c r="R37" s="34"/>
       <c r="S37" s="77">
-        <f t="shared" ref="S37" si="3">SUM(J37:R37)</f>
-        <v>2.8</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="T37" s="15"/>
       <c r="U37" s="84"/>
@@ -3542,7 +3724,7 @@
       </c>
       <c r="R38" s="34"/>
       <c r="S38" s="77">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="T38" s="15"/>
@@ -3587,12 +3769,16 @@
         <v>1</v>
       </c>
       <c r="O39" s="35"/>
-      <c r="P39" s="35"/>
-      <c r="Q39" s="35"/>
+      <c r="P39" s="35">
+        <v>1</v>
+      </c>
+      <c r="Q39" s="35">
+        <v>1</v>
+      </c>
       <c r="R39" s="35"/>
       <c r="S39" s="78">
-        <f t="shared" si="2"/>
-        <v>5</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="T39" s="15"/>
     </row>
@@ -3626,10 +3812,19 @@
       <c r="M40" s="36">
         <v>1</v>
       </c>
+      <c r="N40" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="P40" s="36">
+        <v>1</v>
+      </c>
+      <c r="Q40" s="36">
+        <v>1</v>
+      </c>
       <c r="R40" s="36"/>
       <c r="S40" s="77">
-        <f t="shared" si="2"/>
-        <v>3.75</v>
+        <f t="shared" si="0"/>
+        <v>2.5</v>
       </c>
       <c r="T40" s="15"/>
       <c r="U40" s="15"/>
@@ -3671,12 +3866,16 @@
         <v>0.5</v>
       </c>
       <c r="O41" s="36"/>
-      <c r="P41" s="36"/>
-      <c r="Q41" s="36"/>
+      <c r="P41" s="36">
+        <v>1</v>
+      </c>
+      <c r="Q41" s="36">
+        <v>1</v>
+      </c>
       <c r="R41" s="36"/>
       <c r="S41" s="77">
-        <f t="shared" si="2"/>
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>2.5</v>
       </c>
       <c r="T41" s="15"/>
       <c r="U41" s="3"/>
@@ -3704,9 +3903,12 @@
         <v>1</v>
       </c>
       <c r="M42" s="36"/>
+      <c r="Q42" s="36">
+        <v>1</v>
+      </c>
       <c r="R42" s="36"/>
       <c r="S42" s="77">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="T42" s="15"/>
@@ -3748,10 +3950,16 @@
       <c r="N43" s="36">
         <v>1</v>
       </c>
+      <c r="P43" s="36">
+        <v>1</v>
+      </c>
+      <c r="Q43" s="36">
+        <v>1</v>
+      </c>
       <c r="R43" s="36"/>
       <c r="S43" s="77">
-        <f t="shared" si="2"/>
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="T43" s="15"/>
       <c r="X43" s="6"/>
@@ -3786,10 +3994,16 @@
       <c r="N44" s="36">
         <v>1</v>
       </c>
+      <c r="P44" s="36">
+        <v>1</v>
+      </c>
+      <c r="Q44" s="36">
+        <v>1</v>
+      </c>
       <c r="R44" s="36"/>
       <c r="S44" s="77">
-        <f t="shared" si="2"/>
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="T44" s="15"/>
       <c r="U44" s="15"/>
@@ -3825,10 +4039,16 @@
       <c r="N45" s="36">
         <v>1</v>
       </c>
+      <c r="P45" s="36">
+        <v>1</v>
+      </c>
+      <c r="Q45" s="36">
+        <v>1</v>
+      </c>
       <c r="R45" s="36"/>
       <c r="S45" s="77">
-        <f t="shared" si="2"/>
-        <v>3.75</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="T45" s="15"/>
       <c r="W45" s="6"/>
@@ -3869,12 +4089,16 @@
         <v>1</v>
       </c>
       <c r="O46" s="36"/>
-      <c r="P46" s="36"/>
-      <c r="Q46" s="36"/>
+      <c r="P46" s="36">
+        <v>1</v>
+      </c>
+      <c r="Q46" s="36">
+        <v>1</v>
+      </c>
       <c r="R46" s="36"/>
       <c r="S46" s="77">
-        <f t="shared" si="2"/>
-        <v>5</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="T46" s="15"/>
       <c r="U46" s="3"/>
@@ -3917,9 +4141,15 @@
       <c r="N47" s="36">
         <v>1</v>
       </c>
+      <c r="P47" s="36">
+        <v>1</v>
+      </c>
+      <c r="Q47" s="36">
+        <v>1</v>
+      </c>
       <c r="R47" s="36"/>
       <c r="S47" s="77">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="T47" s="15"/>
@@ -3956,10 +4186,16 @@
       <c r="N48" s="36">
         <v>0.5</v>
       </c>
+      <c r="P48" s="36">
+        <v>0.75</v>
+      </c>
+      <c r="Q48" s="36">
+        <v>1</v>
+      </c>
       <c r="R48" s="34"/>
       <c r="S48" s="77">
-        <f t="shared" si="2"/>
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>2.25</v>
       </c>
       <c r="T48" s="15"/>
     </row>
@@ -3999,12 +4235,16 @@
         <v>0.5</v>
       </c>
       <c r="O49" s="35"/>
-      <c r="P49" s="35"/>
-      <c r="Q49" s="35"/>
+      <c r="P49" s="35">
+        <v>0.75</v>
+      </c>
+      <c r="Q49" s="35">
+        <v>1</v>
+      </c>
       <c r="R49" s="35"/>
       <c r="S49" s="78">
-        <f t="shared" si="2"/>
-        <v>2.5</v>
+        <f t="shared" si="0"/>
+        <v>2.25</v>
       </c>
       <c r="T49" s="15"/>
       <c r="U49" s="15"/>
@@ -4046,10 +4286,16 @@
       <c r="N50" s="36">
         <v>1</v>
       </c>
+      <c r="P50" s="36">
+        <v>1</v>
+      </c>
+      <c r="Q50" s="36">
+        <v>1</v>
+      </c>
       <c r="R50" s="34"/>
       <c r="S50" s="77">
-        <f t="shared" si="2"/>
-        <v>4.7</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="T50" s="15"/>
       <c r="Y50" s="33"/>
@@ -4093,12 +4339,16 @@
         <v>1</v>
       </c>
       <c r="O51" s="36"/>
-      <c r="P51" s="36"/>
-      <c r="Q51" s="36"/>
+      <c r="P51" s="36">
+        <v>1</v>
+      </c>
+      <c r="Q51" s="36">
+        <v>1</v>
+      </c>
       <c r="R51" s="34"/>
       <c r="S51" s="77">
-        <f t="shared" si="2"/>
-        <v>5</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="T51" s="15"/>
       <c r="U51" s="3"/>
@@ -4126,7 +4376,7 @@
       </c>
       <c r="R52" s="34"/>
       <c r="S52" s="77">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
       <c r="T52" s="15"/>
@@ -4145,7 +4395,7 @@
       </c>
       <c r="R53" s="34"/>
       <c r="S53" s="77">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="T53" s="15"/>
@@ -4170,8 +4420,8 @@
       </c>
       <c r="R54" s="34"/>
       <c r="S54" s="77">
-        <f t="shared" si="2"/>
-        <v>0.7</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="T54" s="15"/>
       <c r="W54" s="6"/>
@@ -4209,10 +4459,16 @@
       <c r="N55" s="36">
         <v>1</v>
       </c>
+      <c r="P55" s="36">
+        <v>1</v>
+      </c>
+      <c r="Q55" s="36">
+        <v>1</v>
+      </c>
       <c r="R55" s="34"/>
       <c r="S55" s="77">
-        <f t="shared" si="2"/>
-        <v>5</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="T55" s="15"/>
       <c r="Y55" s="33"/>
@@ -4251,11 +4507,15 @@
         <v>1</v>
       </c>
       <c r="O56" s="35"/>
-      <c r="P56" s="35"/>
-      <c r="Q56" s="35"/>
+      <c r="P56" s="35">
+        <v>1</v>
+      </c>
+      <c r="Q56" s="35">
+        <v>1</v>
+      </c>
       <c r="R56" s="35"/>
       <c r="S56" s="78">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="T56" s="15"/>
@@ -4294,10 +4554,16 @@
       <c r="N57" s="36">
         <v>1</v>
       </c>
+      <c r="P57" s="36">
+        <v>1</v>
+      </c>
+      <c r="Q57" s="36">
+        <v>1</v>
+      </c>
       <c r="R57" s="34"/>
       <c r="S57" s="77">
-        <f t="shared" si="2"/>
-        <v>5</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="T57" s="15"/>
       <c r="Y57" s="33"/>
@@ -4334,10 +4600,16 @@
       <c r="N58" s="36">
         <v>1</v>
       </c>
+      <c r="P58" s="36">
+        <v>1</v>
+      </c>
+      <c r="Q58" s="36">
+        <v>1</v>
+      </c>
       <c r="R58" s="34"/>
       <c r="S58" s="77">
-        <f t="shared" si="2"/>
-        <v>5</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="T58" s="15"/>
       <c r="Y58" s="33"/>
@@ -4358,7 +4630,7 @@
       </c>
       <c r="R59" s="34"/>
       <c r="S59" s="77">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="T59" s="15"/>
@@ -4390,14 +4662,18 @@
         <v>0</v>
       </c>
       <c r="M60" s="12"/>
-      <c r="N60" s="35"/>
-      <c r="O60" s="35"/>
+      <c r="N60" s="35">
+        <v>1</v>
+      </c>
+      <c r="O60" s="35">
+        <v>1</v>
+      </c>
       <c r="P60" s="35"/>
       <c r="Q60" s="35"/>
       <c r="R60" s="35"/>
       <c r="S60" s="78">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="T60" s="15"/>
       <c r="X60" s="6"/>
@@ -4420,10 +4696,16 @@
       <c r="L61" s="2">
         <v>0</v>
       </c>
+      <c r="N61" s="36">
+        <v>1</v>
+      </c>
+      <c r="O61" s="36">
+        <v>1</v>
+      </c>
       <c r="R61" s="34"/>
       <c r="S61" s="77">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="T61" s="15"/>
       <c r="Y61" s="33"/>
@@ -4454,14 +4736,20 @@
         <v>1</v>
       </c>
       <c r="M62" s="12"/>
-      <c r="N62" s="35"/>
+      <c r="N62" s="35">
+        <v>1</v>
+      </c>
       <c r="O62" s="35"/>
-      <c r="P62" s="35"/>
-      <c r="Q62" s="35"/>
+      <c r="P62" s="35">
+        <v>1</v>
+      </c>
+      <c r="Q62" s="35">
+        <v>1</v>
+      </c>
       <c r="R62" s="35"/>
       <c r="S62" s="78">
-        <f t="shared" si="2"/>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="T62" s="15"/>
     </row>
@@ -4481,12 +4769,19 @@
       <c r="L63" s="20">
         <v>1</v>
       </c>
-      <c r="R63" s="36">
-        <v>1</v>
-      </c>
+      <c r="N63" s="36">
+        <v>1</v>
+      </c>
+      <c r="P63" s="36">
+        <v>1</v>
+      </c>
+      <c r="Q63" s="36">
+        <v>1</v>
+      </c>
+      <c r="R63" s="36"/>
       <c r="S63" s="77">
-        <f t="shared" si="2"/>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="T63" s="15"/>
     </row>
@@ -4505,7 +4800,9 @@
       <c r="F64" s="14"/>
       <c r="G64" s="14"/>
       <c r="H64" s="14"/>
-      <c r="I64" s="22"/>
+      <c r="I64" s="22" t="s">
+        <v>189</v>
+      </c>
       <c r="J64" s="36"/>
       <c r="K64" s="2">
         <v>1</v>
@@ -4518,11 +4815,9 @@
       <c r="O64" s="36"/>
       <c r="P64" s="36"/>
       <c r="Q64" s="36"/>
-      <c r="R64" s="34">
-        <v>-2</v>
-      </c>
+      <c r="R64" s="34"/>
       <c r="S64" s="77">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="T64" s="15"/>
@@ -4552,10 +4847,19 @@
       <c r="L65" s="2">
         <v>1</v>
       </c>
+      <c r="N65" s="36">
+        <v>1</v>
+      </c>
+      <c r="P65" s="36">
+        <v>1</v>
+      </c>
+      <c r="Q65" s="36">
+        <v>1</v>
+      </c>
       <c r="R65" s="34"/>
       <c r="S65" s="77">
-        <f t="shared" si="2"/>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="T65" s="15"/>
       <c r="V65" s="33"/>
@@ -4582,12 +4886,14 @@
       <c r="N66" s="36"/>
       <c r="O66" s="36"/>
       <c r="P66" s="36"/>
-      <c r="Q66" s="36"/>
+      <c r="Q66" s="36">
+        <v>1</v>
+      </c>
       <c r="R66" s="34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S66" s="77">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="T66" s="15"/>
@@ -4616,10 +4922,16 @@
       <c r="N67" s="36">
         <v>1</v>
       </c>
+      <c r="P67" s="36">
+        <v>1</v>
+      </c>
+      <c r="Q67" s="36">
+        <v>1</v>
+      </c>
       <c r="R67" s="34"/>
       <c r="S67" s="77">
-        <f t="shared" ref="S67:S98" si="4">SUM(J67:R67)</f>
-        <v>2</v>
+        <f t="shared" ref="S67:S69" si="4">SUM(N67:R67)</f>
+        <v>3</v>
       </c>
       <c r="T67" s="15"/>
       <c r="Y67" s="6"/>
@@ -4644,10 +4956,19 @@
       <c r="L68" s="2">
         <v>1</v>
       </c>
+      <c r="N68" s="36">
+        <v>1</v>
+      </c>
+      <c r="P68" s="36">
+        <v>1</v>
+      </c>
+      <c r="Q68" s="36">
+        <v>1</v>
+      </c>
       <c r="R68" s="34"/>
       <c r="S68" s="77">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="T68" s="15"/>
     </row>
@@ -4679,10 +5000,12 @@
       <c r="O69" s="37"/>
       <c r="P69" s="37"/>
       <c r="Q69" s="37"/>
-      <c r="R69" s="37"/>
+      <c r="R69" s="37">
+        <v>2</v>
+      </c>
       <c r="S69" s="79">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T69" s="15"/>
       <c r="U69" s="3"/>
@@ -4703,26 +5026,26 @@
         <v>98</v>
       </c>
       <c r="J71" s="85"/>
-      <c r="K71" s="65">
-        <f t="array" ref="K71">SUM($C2:$C69*(K2:K69&gt;=0.9)*($S2:$S69&gt;=$U$12))</f>
-        <v>184</v>
-      </c>
-      <c r="L71" s="65">
-        <f t="array" ref="L71">SUM($C2:$C69*(L2:L69&gt;=0.9)*($S2:$S69&gt;=$U$12))</f>
-        <v>111</v>
-      </c>
-      <c r="M71" s="65">
-        <f t="array" ref="M71">SUM($C2:$C69*(M2:M69&gt;=0.9)*($S2:$S69&gt;=$U$12))</f>
-        <v>200</v>
-      </c>
-      <c r="N71" s="85"/>
-      <c r="O71" s="65"/>
-      <c r="P71" s="65"/>
-      <c r="Q71" s="65"/>
-      <c r="R71" s="66">
-        <f t="array" ref="R71">SUM($C2:$C69*(R2:R69&gt;=0.9)*($S2:$S69&gt;=$U$12))</f>
-        <v>8</v>
-      </c>
+      <c r="K71" s="65"/>
+      <c r="L71" s="65"/>
+      <c r="M71" s="65"/>
+      <c r="N71" s="65">
+        <f t="array" ref="N71">SUM($C2:$C69*(N2:N69&gt;=0.9)*($S2:$S69&gt;=$U$12))</f>
+        <v>191</v>
+      </c>
+      <c r="O71" s="65">
+        <f t="array" ref="O71">SUM($C2:$C69*(O2:O69&gt;=0.9)*($S2:$S69&gt;=$U$12))</f>
+        <v>14</v>
+      </c>
+      <c r="P71" s="65">
+        <f t="array" ref="P71">SUM($C2:$C69*(P2:P69&gt;=0.9)*($S2:$S69&gt;=$U$12))</f>
+        <v>187</v>
+      </c>
+      <c r="Q71" s="65">
+        <f t="array" ref="Q71">SUM($C2:$C69*(Q2:Q69&gt;=0.9)*($S2:$S69&gt;=$U$12))</f>
+        <v>227</v>
+      </c>
+      <c r="R71" s="66"/>
       <c r="T71" s="15"/>
       <c r="W71" s="33"/>
     </row>
@@ -4731,26 +5054,26 @@
         <v>100</v>
       </c>
       <c r="J72" s="86"/>
-      <c r="K72" s="68">
-        <f t="array" ref="K72">SUM($C2:$C69*K2:K69*($S2:$S69&gt;=$U$12))</f>
-        <v>189</v>
-      </c>
-      <c r="L72" s="68">
-        <f t="array" ref="L72">SUM($C2:$C69*L2:L69*($S2:$S69&gt;=$U$12))</f>
-        <v>168.25000000000003</v>
-      </c>
-      <c r="M72" s="68">
-        <f t="array" ref="M72">SUM($C2:$C69*M2:M69*($S2:$S69&gt;=$U$12))</f>
-        <v>200</v>
-      </c>
-      <c r="N72" s="86"/>
-      <c r="O72" s="68"/>
-      <c r="P72" s="68"/>
-      <c r="Q72" s="68"/>
-      <c r="R72" s="69">
-        <f t="array" ref="R72">SUM($C2:$C69*R2:R69*($S2:$S69&gt;=$U$12))</f>
-        <v>9</v>
-      </c>
+      <c r="K72" s="68"/>
+      <c r="L72" s="68"/>
+      <c r="M72" s="68"/>
+      <c r="N72" s="68">
+        <f t="array" ref="N72">SUM($C2:$C69*N2:N69*($S2:$S69&gt;=$U$12))</f>
+        <v>201</v>
+      </c>
+      <c r="O72" s="68">
+        <f t="array" ref="O72">SUM($C2:$C69*O2:O69*($S2:$S69&gt;=$U$12))</f>
+        <v>14</v>
+      </c>
+      <c r="P72" s="68">
+        <f t="array" ref="P72">SUM($C2:$C69*P2:P69*($S2:$S69&gt;=$U$12))</f>
+        <v>210.5</v>
+      </c>
+      <c r="Q72" s="68">
+        <f t="array" ref="Q72">SUM($C2:$C69*Q2:Q69*($S2:$S69&gt;=$U$12))</f>
+        <v>227</v>
+      </c>
+      <c r="R72" s="69"/>
       <c r="T72" s="15"/>
       <c r="Y72" s="6"/>
       <c r="Z72" s="6"/>
@@ -4762,26 +5085,26 @@
         <v>99</v>
       </c>
       <c r="J73" s="86"/>
-      <c r="K73" s="68">
-        <f t="array" ref="K73">SUM($C$2:$C$69*(K$2:K$69&gt;=0.1)*($S$2:$S$69&gt;=$U$12))</f>
-        <v>194</v>
-      </c>
-      <c r="L73" s="68">
-        <f t="array" ref="L73">SUM($C$2:$C$69*(L$2:L$69&gt;=0.1)*($S$2:$S$69&gt;=$U$12))</f>
-        <v>204</v>
-      </c>
-      <c r="M73" s="68">
-        <f t="array" ref="M73">SUM($C$2:$C$69*(M$2:M$69&gt;=0.1)*($S$2:$S$69&gt;=$U$12))</f>
-        <v>200</v>
-      </c>
-      <c r="N73" s="86"/>
-      <c r="O73" s="68"/>
-      <c r="P73" s="68"/>
-      <c r="Q73" s="68"/>
-      <c r="R73" s="69">
-        <f t="array" ref="R73">SUM($C$2:$C$69*(R$2:R$69&gt;=0.1)*($S$2:$S$69&gt;=$U$12))</f>
-        <v>8</v>
-      </c>
+      <c r="K73" s="68"/>
+      <c r="L73" s="68"/>
+      <c r="M73" s="68"/>
+      <c r="N73" s="68">
+        <f t="array" ref="N73">SUM($C$2:$C$69*(N$2:N$69&gt;=0.1)*($S$2:$S$69&gt;=$U$12))</f>
+        <v>211</v>
+      </c>
+      <c r="O73" s="68">
+        <f t="array" ref="O73">SUM($C$2:$C$69*(O$2:O$69&gt;=0.1)*($S$2:$S$69&gt;=$U$12))</f>
+        <v>14</v>
+      </c>
+      <c r="P73" s="68">
+        <f t="array" ref="P73">SUM($C$2:$C$69*(P$2:P$69&gt;=0.1)*($S$2:$S$69&gt;=$U$12))</f>
+        <v>224</v>
+      </c>
+      <c r="Q73" s="68">
+        <f t="array" ref="Q73">SUM($C$2:$C$69*(Q$2:Q$69&gt;=0.1)*($S$2:$S$69&gt;=$U$12))</f>
+        <v>227</v>
+      </c>
+      <c r="R73" s="69"/>
       <c r="T73" s="15"/>
     </row>
     <row r="74" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -4797,26 +5120,26 @@
         <v>101</v>
       </c>
       <c r="J74" s="86"/>
-      <c r="K74" s="68">
-        <f>LOOKUP($U$12,$U23:$U31,$V23:$V31)</f>
-        <v>223</v>
-      </c>
-      <c r="L74" s="68">
-        <f>LOOKUP($U$12,$U23:$U31,$V23:$V31)</f>
-        <v>223</v>
-      </c>
-      <c r="M74" s="68">
-        <f>LOOKUP($U$12,$U23:$U31,$V23:$V31)</f>
-        <v>223</v>
-      </c>
-      <c r="N74" s="86"/>
-      <c r="O74" s="68"/>
-      <c r="P74" s="68"/>
-      <c r="Q74" s="68"/>
-      <c r="R74" s="69">
-        <f>LOOKUP($U$12,$U23:$U31,$V23:$V31)</f>
-        <v>223</v>
-      </c>
+      <c r="K74" s="68"/>
+      <c r="L74" s="68"/>
+      <c r="M74" s="68"/>
+      <c r="N74" s="68">
+        <f t="shared" ref="N74:Q74" si="5">LOOKUP($U$12,$U23:$U31,$V23:$V31)</f>
+        <v>241</v>
+      </c>
+      <c r="O74" s="68">
+        <f t="shared" si="5"/>
+        <v>241</v>
+      </c>
+      <c r="P74" s="68">
+        <f t="shared" si="5"/>
+        <v>241</v>
+      </c>
+      <c r="Q74" s="68">
+        <f t="shared" si="5"/>
+        <v>241</v>
+      </c>
+      <c r="R74" s="69"/>
       <c r="S74" s="3"/>
       <c r="T74" s="15"/>
       <c r="U74" s="3"/>
@@ -4833,26 +5156,26 @@
         <v>102</v>
       </c>
       <c r="J75" s="86"/>
-      <c r="K75" s="70">
-        <f t="shared" ref="K75:R75" si="5">K72/K74</f>
-        <v>0.84753363228699552</v>
-      </c>
-      <c r="L75" s="70">
-        <f t="shared" si="5"/>
-        <v>0.75448430493273555</v>
-      </c>
-      <c r="M75" s="70">
-        <f t="shared" si="5"/>
-        <v>0.89686098654708524</v>
-      </c>
-      <c r="N75" s="86"/>
-      <c r="O75" s="70"/>
-      <c r="P75" s="70"/>
-      <c r="Q75" s="70"/>
-      <c r="R75" s="71">
-        <f t="shared" si="5"/>
-        <v>4.0358744394618833E-2</v>
-      </c>
+      <c r="K75" s="70"/>
+      <c r="L75" s="70"/>
+      <c r="M75" s="70"/>
+      <c r="N75" s="70">
+        <f t="shared" ref="N75:Q75" si="6">N72/N74</f>
+        <v>0.8340248962655602</v>
+      </c>
+      <c r="O75" s="70">
+        <f t="shared" si="6"/>
+        <v>5.8091286307053944E-2</v>
+      </c>
+      <c r="P75" s="70">
+        <f t="shared" si="6"/>
+        <v>0.87344398340248963</v>
+      </c>
+      <c r="Q75" s="70">
+        <f t="shared" si="6"/>
+        <v>0.94190871369294604</v>
+      </c>
+      <c r="R75" s="71"/>
       <c r="T75" s="15"/>
       <c r="Y75" s="6"/>
       <c r="Z75" s="6"/>
@@ -4865,26 +5188,26 @@
         <v>80</v>
       </c>
       <c r="J76" s="87"/>
-      <c r="K76" s="73">
-        <f t="array" ref="K76">SUM($C2:$C69*K2:K69*($S2:$S69&lt;$U$12))</f>
+      <c r="K76" s="73"/>
+      <c r="L76" s="73"/>
+      <c r="M76" s="73"/>
+      <c r="N76" s="73">
+        <f t="array" ref="N76">SUM($C2:$C69*N2:N69*($S2:$S69&lt;$U$12))</f>
+        <v>1.5</v>
+      </c>
+      <c r="O76" s="73">
+        <f t="array" ref="O76">SUM($C2:$C69*O2:O69*($S2:$S69&lt;$U$12))</f>
+        <v>0</v>
+      </c>
+      <c r="P76" s="73">
+        <f t="array" ref="P76">SUM($C2:$C69*P2:P69*($S2:$S69&lt;$U$12))</f>
+        <v>0.5</v>
+      </c>
+      <c r="Q76" s="73">
+        <f t="array" ref="Q76">SUM($C2:$C69*Q2:Q69*($S2:$S69&lt;$U$12))</f>
         <v>6</v>
       </c>
-      <c r="L76" s="73">
-        <f t="array" ref="L76">SUM($C2:$C69*L2:L69*($S2:$S69&lt;$U$12))</f>
-        <v>21.849999999999998</v>
-      </c>
-      <c r="M76" s="73">
-        <f t="array" ref="M76">SUM($C2:$C69*M2:M69*($S2:$S69&lt;$U$12))</f>
-        <v>0</v>
-      </c>
-      <c r="N76" s="87"/>
-      <c r="O76" s="73"/>
-      <c r="P76" s="73"/>
-      <c r="Q76" s="73"/>
-      <c r="R76" s="74">
-        <f t="array" ref="R76">SUM($C2:$C69*R2:R69*($S2:$S69&lt;$U$12))</f>
-        <v>-4</v>
-      </c>
+      <c r="R76" s="74"/>
       <c r="T76" s="15"/>
     </row>
     <row r="77" spans="1:28" x14ac:dyDescent="0.3">
@@ -5015,14 +5338,36 @@
       <c r="AB112" s="33"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:S69">
-    <cfRule type="expression" dxfId="2" priority="31" stopIfTrue="1">
+  <conditionalFormatting sqref="B2:M69 O2:O69 Q2:S69">
+    <cfRule type="expression" dxfId="8" priority="37" stopIfTrue="1">
       <formula>$S2&gt;=(0.5+$U$12)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="38" stopIfTrue="1">
       <formula>$S2&gt;=$U$12</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="33">
+    <cfRule type="expression" dxfId="6" priority="39">
+      <formula>$S2&gt;=($U$12-0.5)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N2:N69">
+    <cfRule type="expression" dxfId="5" priority="4" stopIfTrue="1">
+      <formula>$S2&gt;=(0.5+$U$12)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="5" stopIfTrue="1">
+      <formula>$S2&gt;=$U$12</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="6">
+      <formula>$S2&gt;=($U$12-0.5)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P2:P69">
+    <cfRule type="expression" dxfId="2" priority="1" stopIfTrue="1">
+      <formula>$S2&gt;=(0.5+$U$12)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
+      <formula>$S2&gt;=$U$12</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="3">
       <formula>$S2&gt;=($U$12-0.5)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>